<commit_message>
Update OSG ILP List of participants (20250401).xlsx
</commit_message>
<xml_diff>
--- a/frontend/public/external/OSG ILP List of participants (20250401).xlsx
+++ b/frontend/public/external/OSG ILP List of participants (20250401).xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moseslee/Desktop/ecss-cms/frontend/public/external/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC04CE1-B348-B843-9174-8DF394D36A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3567E8D-7ABF-E041-B2C3-EBCD09C8AE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3920" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="3040" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOP" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Email</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Others</t>
-  </si>
-  <si>
-    <t>Receipt No / SF Invoice No</t>
   </si>
   <si>
     <t>*Course Title</t>
@@ -752,7 +749,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -817,9 +814,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -990,33 +984,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1042,8 +1009,35 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1068,14 +1062,14 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="gray125">
-          <bgColor auto="1"/>
-        </patternFill>
+        <patternFill patternType="gray125"/>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="gray125"/>
+        <patternFill patternType="gray125">
+          <bgColor auto="1"/>
+        </patternFill>
       </fill>
     </dxf>
   </dxfs>
@@ -1650,10 +1644,10 @@
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q153"/>
+  <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q1:W1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1670,18 +1664,17 @@
     <col min="11" max="14" width="35.1640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="26.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="37.6640625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="1"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:17" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1701,59 +1694,59 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:17" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
       <c r="H5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="77"/>
+      <c r="I5" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="76"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="24"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="23"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>24</v>
+    <row r="6" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1764,55 +1757,55 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="29"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="28"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:17" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="80" t="s">
+    <row r="7" spans="1:16" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-    </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="58.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>1</v>
@@ -1824,28 +1817,25 @@
         <v>8</v>
       </c>
       <c r="K8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="M8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1856,15 +1846,14 @@
       <c r="H9" s="16"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
-      <c r="Q9" s="16"/>
-    </row>
-    <row r="10" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1875,15 +1864,14 @@
       <c r="H10" s="16"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
-      <c r="Q10" s="16"/>
-    </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1900,9 +1888,8 @@
       <c r="N11" s="18"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
-      <c r="Q11" s="16"/>
-    </row>
-    <row r="12" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1919,9 +1906,8 @@
       <c r="N12" s="18"/>
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
-      <c r="Q12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1932,15 +1918,14 @@
       <c r="H13" s="16"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
-      <c r="Q13" s="16"/>
-    </row>
-    <row r="14" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1951,15 +1936,14 @@
       <c r="H14" s="16"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
       <c r="O14" s="19"/>
       <c r="P14" s="19"/>
-      <c r="Q14" s="16"/>
-    </row>
-    <row r="15" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1976,9 +1960,8 @@
       <c r="N15" s="18"/>
       <c r="O15" s="19"/>
       <c r="P15" s="19"/>
-      <c r="Q15" s="16"/>
-    </row>
-    <row r="16" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1995,9 +1978,8 @@
       <c r="N16" s="18"/>
       <c r="O16" s="19"/>
       <c r="P16" s="19"/>
-      <c r="Q16" s="16"/>
-    </row>
-    <row r="17" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2014,9 +1996,8 @@
       <c r="N17" s="18"/>
       <c r="O17" s="16"/>
       <c r="P17" s="19"/>
-      <c r="Q17" s="16"/>
-    </row>
-    <row r="18" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2033,9 +2014,8 @@
       <c r="N18" s="18"/>
       <c r="O18" s="16"/>
       <c r="P18" s="19"/>
-      <c r="Q18" s="16"/>
-    </row>
-    <row r="19" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2052,9 +2032,8 @@
       <c r="N19" s="18"/>
       <c r="O19" s="16"/>
       <c r="P19" s="19"/>
-      <c r="Q19" s="16"/>
-    </row>
-    <row r="20" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2071,9 +2050,8 @@
       <c r="N20" s="18"/>
       <c r="O20" s="16"/>
       <c r="P20" s="19"/>
-      <c r="Q20" s="16"/>
-    </row>
-    <row r="21" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2090,9 +2068,8 @@
       <c r="N21" s="18"/>
       <c r="O21" s="16"/>
       <c r="P21" s="19"/>
-      <c r="Q21" s="16"/>
-    </row>
-    <row r="22" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2109,9 +2086,8 @@
       <c r="N22" s="18"/>
       <c r="O22" s="16"/>
       <c r="P22" s="19"/>
-      <c r="Q22" s="16"/>
-    </row>
-    <row r="23" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2128,9 +2104,8 @@
       <c r="N23" s="18"/>
       <c r="O23" s="16"/>
       <c r="P23" s="19"/>
-      <c r="Q23" s="16"/>
-    </row>
-    <row r="24" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2147,9 +2122,8 @@
       <c r="N24" s="18"/>
       <c r="O24" s="16"/>
       <c r="P24" s="19"/>
-      <c r="Q24" s="16"/>
-    </row>
-    <row r="25" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2166,9 +2140,8 @@
       <c r="N25" s="18"/>
       <c r="O25" s="16"/>
       <c r="P25" s="19"/>
-      <c r="Q25" s="16"/>
-    </row>
-    <row r="26" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2185,9 +2158,8 @@
       <c r="N26" s="18"/>
       <c r="O26" s="16"/>
       <c r="P26" s="19"/>
-      <c r="Q26" s="16"/>
-    </row>
-    <row r="27" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2204,9 +2176,8 @@
       <c r="N27" s="18"/>
       <c r="O27" s="19"/>
       <c r="P27" s="19"/>
-      <c r="Q27" s="16"/>
-    </row>
-    <row r="28" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2223,9 +2194,8 @@
       <c r="N28" s="18"/>
       <c r="O28" s="19"/>
       <c r="P28" s="19"/>
-      <c r="Q28" s="16"/>
-    </row>
-    <row r="29" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2242,9 +2212,8 @@
       <c r="N29" s="18"/>
       <c r="O29" s="19"/>
       <c r="P29" s="19"/>
-      <c r="Q29" s="16"/>
-    </row>
-    <row r="30" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -2261,9 +2230,8 @@
       <c r="N30" s="18"/>
       <c r="O30" s="19"/>
       <c r="P30" s="19"/>
-      <c r="Q30" s="16"/>
-    </row>
-    <row r="31" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -2280,9 +2248,8 @@
       <c r="N31" s="18"/>
       <c r="O31" s="19"/>
       <c r="P31" s="19"/>
-      <c r="Q31" s="16"/>
-    </row>
-    <row r="32" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -2299,9 +2266,8 @@
       <c r="N32" s="18"/>
       <c r="O32" s="19"/>
       <c r="P32" s="19"/>
-      <c r="Q32" s="16"/>
-    </row>
-    <row r="33" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -2318,9 +2284,8 @@
       <c r="N33" s="18"/>
       <c r="O33" s="19"/>
       <c r="P33" s="19"/>
-      <c r="Q33" s="16"/>
-    </row>
-    <row r="34" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -2337,9 +2302,8 @@
       <c r="N34" s="18"/>
       <c r="O34" s="19"/>
       <c r="P34" s="19"/>
-      <c r="Q34" s="16"/>
-    </row>
-    <row r="35" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -2356,9 +2320,8 @@
       <c r="N35" s="18"/>
       <c r="O35" s="19"/>
       <c r="P35" s="19"/>
-      <c r="Q35" s="16"/>
-    </row>
-    <row r="36" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -2375,9 +2338,8 @@
       <c r="N36" s="18"/>
       <c r="O36" s="19"/>
       <c r="P36" s="19"/>
-      <c r="Q36" s="16"/>
-    </row>
-    <row r="37" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -2394,9 +2356,8 @@
       <c r="N37" s="18"/>
       <c r="O37" s="19"/>
       <c r="P37" s="19"/>
-      <c r="Q37" s="16"/>
-    </row>
-    <row r="38" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -2413,9 +2374,8 @@
       <c r="N38" s="18"/>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
-      <c r="Q38" s="16"/>
-    </row>
-    <row r="39" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -2432,9 +2392,8 @@
       <c r="N39" s="18"/>
       <c r="O39" s="19"/>
       <c r="P39" s="19"/>
-      <c r="Q39" s="16"/>
-    </row>
-    <row r="40" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -2451,9 +2410,8 @@
       <c r="N40" s="18"/>
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
-      <c r="Q40" s="16"/>
-    </row>
-    <row r="41" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -2470,9 +2428,8 @@
       <c r="N41" s="18"/>
       <c r="O41" s="19"/>
       <c r="P41" s="19"/>
-      <c r="Q41" s="16"/>
-    </row>
-    <row r="42" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -2489,9 +2446,8 @@
       <c r="N42" s="18"/>
       <c r="O42" s="19"/>
       <c r="P42" s="19"/>
-      <c r="Q42" s="16"/>
-    </row>
-    <row r="43" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -2508,9 +2464,8 @@
       <c r="N43" s="18"/>
       <c r="O43" s="19"/>
       <c r="P43" s="19"/>
-      <c r="Q43" s="16"/>
-    </row>
-    <row r="44" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -2527,9 +2482,8 @@
       <c r="N44" s="18"/>
       <c r="O44" s="19"/>
       <c r="P44" s="19"/>
-      <c r="Q44" s="16"/>
-    </row>
-    <row r="45" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -2546,9 +2500,8 @@
       <c r="N45" s="18"/>
       <c r="O45" s="19"/>
       <c r="P45" s="19"/>
-      <c r="Q45" s="16"/>
-    </row>
-    <row r="46" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -2565,9 +2518,8 @@
       <c r="N46" s="18"/>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
-      <c r="Q46" s="16"/>
-    </row>
-    <row r="47" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -2584,9 +2536,8 @@
       <c r="N47" s="18"/>
       <c r="O47" s="19"/>
       <c r="P47" s="19"/>
-      <c r="Q47" s="16"/>
-    </row>
-    <row r="48" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -2603,9 +2554,8 @@
       <c r="N48" s="18"/>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
-      <c r="Q48" s="16"/>
-    </row>
-    <row r="49" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
@@ -2622,9 +2572,8 @@
       <c r="N49" s="18"/>
       <c r="O49" s="19"/>
       <c r="P49" s="19"/>
-      <c r="Q49" s="16"/>
-    </row>
-    <row r="50" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
       <c r="B50" s="16"/>
       <c r="C50" s="16"/>
@@ -2641,9 +2590,8 @@
       <c r="N50" s="18"/>
       <c r="O50" s="19"/>
       <c r="P50" s="19"/>
-      <c r="Q50" s="16"/>
-    </row>
-    <row r="51" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -2660,9 +2608,8 @@
       <c r="N51" s="18"/>
       <c r="O51" s="19"/>
       <c r="P51" s="19"/>
-      <c r="Q51" s="16"/>
-    </row>
-    <row r="52" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -2679,9 +2626,8 @@
       <c r="N52" s="18"/>
       <c r="O52" s="19"/>
       <c r="P52" s="19"/>
-      <c r="Q52" s="16"/>
-    </row>
-    <row r="53" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="16"/>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
@@ -2698,9 +2644,8 @@
       <c r="N53" s="18"/>
       <c r="O53" s="19"/>
       <c r="P53" s="19"/>
-      <c r="Q53" s="16"/>
-    </row>
-    <row r="54" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
@@ -2717,9 +2662,8 @@
       <c r="N54" s="18"/>
       <c r="O54" s="19"/>
       <c r="P54" s="19"/>
-      <c r="Q54" s="16"/>
-    </row>
-    <row r="55" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="16"/>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
@@ -2736,9 +2680,8 @@
       <c r="N55" s="18"/>
       <c r="O55" s="19"/>
       <c r="P55" s="19"/>
-      <c r="Q55" s="16"/>
-    </row>
-    <row r="56" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
@@ -2755,9 +2698,8 @@
       <c r="N56" s="18"/>
       <c r="O56" s="19"/>
       <c r="P56" s="19"/>
-      <c r="Q56" s="16"/>
-    </row>
-    <row r="57" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
@@ -2774,9 +2716,8 @@
       <c r="N57" s="18"/>
       <c r="O57" s="19"/>
       <c r="P57" s="19"/>
-      <c r="Q57" s="16"/>
-    </row>
-    <row r="58" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -2793,9 +2734,8 @@
       <c r="N58" s="18"/>
       <c r="O58" s="19"/>
       <c r="P58" s="19"/>
-      <c r="Q58" s="16"/>
-    </row>
-    <row r="59" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
@@ -2812,9 +2752,8 @@
       <c r="N59" s="18"/>
       <c r="O59" s="19"/>
       <c r="P59" s="19"/>
-      <c r="Q59" s="16"/>
-    </row>
-    <row r="60" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
@@ -2831,9 +2770,8 @@
       <c r="N60" s="18"/>
       <c r="O60" s="19"/>
       <c r="P60" s="19"/>
-      <c r="Q60" s="16"/>
-    </row>
-    <row r="61" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="16"/>
@@ -2850,9 +2788,8 @@
       <c r="N61" s="18"/>
       <c r="O61" s="19"/>
       <c r="P61" s="19"/>
-      <c r="Q61" s="16"/>
-    </row>
-    <row r="62" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
@@ -2869,9 +2806,8 @@
       <c r="N62" s="18"/>
       <c r="O62" s="19"/>
       <c r="P62" s="19"/>
-      <c r="Q62" s="16"/>
-    </row>
-    <row r="63" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="16"/>
       <c r="C63" s="16"/>
@@ -2888,9 +2824,8 @@
       <c r="N63" s="18"/>
       <c r="O63" s="19"/>
       <c r="P63" s="19"/>
-      <c r="Q63" s="16"/>
-    </row>
-    <row r="64" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="16"/>
@@ -2907,9 +2842,8 @@
       <c r="N64" s="18"/>
       <c r="O64" s="19"/>
       <c r="P64" s="19"/>
-      <c r="Q64" s="16"/>
-    </row>
-    <row r="65" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
       <c r="B65" s="16"/>
       <c r="C65" s="16"/>
@@ -2926,9 +2860,8 @@
       <c r="N65" s="18"/>
       <c r="O65" s="19"/>
       <c r="P65" s="19"/>
-      <c r="Q65" s="16"/>
-    </row>
-    <row r="66" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
@@ -2945,9 +2878,8 @@
       <c r="N66" s="18"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
-      <c r="Q66" s="16"/>
-    </row>
-    <row r="67" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16"/>
       <c r="B67" s="16"/>
       <c r="C67" s="16"/>
@@ -2964,9 +2896,8 @@
       <c r="N67" s="18"/>
       <c r="O67" s="19"/>
       <c r="P67" s="19"/>
-      <c r="Q67" s="16"/>
-    </row>
-    <row r="68" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="16"/>
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
@@ -2983,9 +2914,8 @@
       <c r="N68" s="18"/>
       <c r="O68" s="19"/>
       <c r="P68" s="19"/>
-      <c r="Q68" s="16"/>
-    </row>
-    <row r="69" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
       <c r="B69" s="16"/>
       <c r="C69" s="16"/>
@@ -3002,9 +2932,8 @@
       <c r="N69" s="18"/>
       <c r="O69" s="19"/>
       <c r="P69" s="19"/>
-      <c r="Q69" s="16"/>
-    </row>
-    <row r="70" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
       <c r="B70" s="16"/>
       <c r="C70" s="16"/>
@@ -3021,9 +2950,8 @@
       <c r="N70" s="18"/>
       <c r="O70" s="19"/>
       <c r="P70" s="19"/>
-      <c r="Q70" s="16"/>
-    </row>
-    <row r="71" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16"/>
       <c r="B71" s="16"/>
       <c r="C71" s="16"/>
@@ -3040,9 +2968,8 @@
       <c r="N71" s="18"/>
       <c r="O71" s="19"/>
       <c r="P71" s="19"/>
-      <c r="Q71" s="16"/>
-    </row>
-    <row r="72" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
       <c r="B72" s="16"/>
       <c r="C72" s="16"/>
@@ -3059,9 +2986,8 @@
       <c r="N72" s="18"/>
       <c r="O72" s="19"/>
       <c r="P72" s="19"/>
-      <c r="Q72" s="16"/>
-    </row>
-    <row r="73" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16"/>
       <c r="B73" s="16"/>
       <c r="C73" s="16"/>
@@ -3078,9 +3004,8 @@
       <c r="N73" s="18"/>
       <c r="O73" s="19"/>
       <c r="P73" s="19"/>
-      <c r="Q73" s="16"/>
-    </row>
-    <row r="74" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
       <c r="C74" s="16"/>
@@ -3097,9 +3022,8 @@
       <c r="N74" s="18"/>
       <c r="O74" s="19"/>
       <c r="P74" s="19"/>
-      <c r="Q74" s="16"/>
-    </row>
-    <row r="75" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
       <c r="B75" s="16"/>
       <c r="C75" s="16"/>
@@ -3116,9 +3040,8 @@
       <c r="N75" s="18"/>
       <c r="O75" s="19"/>
       <c r="P75" s="19"/>
-      <c r="Q75" s="16"/>
-    </row>
-    <row r="76" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -3135,9 +3058,8 @@
       <c r="N76" s="18"/>
       <c r="O76" s="19"/>
       <c r="P76" s="19"/>
-      <c r="Q76" s="16"/>
-    </row>
-    <row r="77" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
       <c r="B77" s="16"/>
       <c r="C77" s="16"/>
@@ -3154,9 +3076,8 @@
       <c r="N77" s="18"/>
       <c r="O77" s="19"/>
       <c r="P77" s="19"/>
-      <c r="Q77" s="16"/>
-    </row>
-    <row r="78" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
@@ -3173,9 +3094,8 @@
       <c r="N78" s="18"/>
       <c r="O78" s="19"/>
       <c r="P78" s="19"/>
-      <c r="Q78" s="16"/>
-    </row>
-    <row r="79" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16"/>
       <c r="B79" s="16"/>
       <c r="C79" s="16"/>
@@ -3192,9 +3112,8 @@
       <c r="N79" s="18"/>
       <c r="O79" s="19"/>
       <c r="P79" s="19"/>
-      <c r="Q79" s="16"/>
-    </row>
-    <row r="80" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="16"/>
       <c r="C80" s="16"/>
@@ -3211,9 +3130,8 @@
       <c r="N80" s="18"/>
       <c r="O80" s="19"/>
       <c r="P80" s="19"/>
-      <c r="Q80" s="16"/>
-    </row>
-    <row r="81" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16"/>
       <c r="B81" s="16"/>
       <c r="C81" s="16"/>
@@ -3230,9 +3148,8 @@
       <c r="N81" s="18"/>
       <c r="O81" s="19"/>
       <c r="P81" s="19"/>
-      <c r="Q81" s="16"/>
-    </row>
-    <row r="82" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
@@ -3249,9 +3166,8 @@
       <c r="N82" s="18"/>
       <c r="O82" s="19"/>
       <c r="P82" s="19"/>
-      <c r="Q82" s="16"/>
-    </row>
-    <row r="83" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -3268,9 +3184,8 @@
       <c r="N83" s="18"/>
       <c r="O83" s="19"/>
       <c r="P83" s="19"/>
-      <c r="Q83" s="16"/>
-    </row>
-    <row r="84" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="16"/>
       <c r="C84" s="16"/>
@@ -3287,9 +3202,8 @@
       <c r="N84" s="18"/>
       <c r="O84" s="19"/>
       <c r="P84" s="19"/>
-      <c r="Q84" s="16"/>
-    </row>
-    <row r="85" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
       <c r="B85" s="16"/>
       <c r="C85" s="16"/>
@@ -3306,9 +3220,8 @@
       <c r="N85" s="18"/>
       <c r="O85" s="19"/>
       <c r="P85" s="19"/>
-      <c r="Q85" s="16"/>
-    </row>
-    <row r="86" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16"/>
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
@@ -3325,9 +3238,8 @@
       <c r="N86" s="18"/>
       <c r="O86" s="19"/>
       <c r="P86" s="19"/>
-      <c r="Q86" s="16"/>
-    </row>
-    <row r="87" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="16"/>
       <c r="C87" s="16"/>
@@ -3344,9 +3256,8 @@
       <c r="N87" s="18"/>
       <c r="O87" s="19"/>
       <c r="P87" s="19"/>
-      <c r="Q87" s="16"/>
-    </row>
-    <row r="88" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
@@ -3363,9 +3274,8 @@
       <c r="N88" s="18"/>
       <c r="O88" s="19"/>
       <c r="P88" s="19"/>
-      <c r="Q88" s="16"/>
-    </row>
-    <row r="89" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16"/>
       <c r="B89" s="16"/>
       <c r="C89" s="16"/>
@@ -3382,9 +3292,8 @@
       <c r="N89" s="18"/>
       <c r="O89" s="19"/>
       <c r="P89" s="19"/>
-      <c r="Q89" s="16"/>
-    </row>
-    <row r="90" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16"/>
       <c r="B90" s="16"/>
       <c r="C90" s="16"/>
@@ -3401,9 +3310,8 @@
       <c r="N90" s="18"/>
       <c r="O90" s="19"/>
       <c r="P90" s="19"/>
-      <c r="Q90" s="16"/>
-    </row>
-    <row r="91" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
@@ -3420,9 +3328,8 @@
       <c r="N91" s="18"/>
       <c r="O91" s="19"/>
       <c r="P91" s="19"/>
-      <c r="Q91" s="16"/>
-    </row>
-    <row r="92" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
       <c r="B92" s="16"/>
       <c r="C92" s="16"/>
@@ -3439,9 +3346,8 @@
       <c r="N92" s="18"/>
       <c r="O92" s="19"/>
       <c r="P92" s="19"/>
-      <c r="Q92" s="16"/>
-    </row>
-    <row r="93" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
       <c r="C93" s="16"/>
@@ -3458,9 +3364,8 @@
       <c r="N93" s="18"/>
       <c r="O93" s="19"/>
       <c r="P93" s="19"/>
-      <c r="Q93" s="16"/>
-    </row>
-    <row r="94" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16"/>
       <c r="B94" s="16"/>
       <c r="C94" s="16"/>
@@ -3477,9 +3382,8 @@
       <c r="N94" s="18"/>
       <c r="O94" s="19"/>
       <c r="P94" s="19"/>
-      <c r="Q94" s="16"/>
-    </row>
-    <row r="95" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
       <c r="B95" s="16"/>
       <c r="C95" s="16"/>
@@ -3496,9 +3400,8 @@
       <c r="N95" s="18"/>
       <c r="O95" s="19"/>
       <c r="P95" s="19"/>
-      <c r="Q95" s="16"/>
-    </row>
-    <row r="96" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
       <c r="B96" s="16"/>
       <c r="C96" s="16"/>
@@ -3515,9 +3418,8 @@
       <c r="N96" s="18"/>
       <c r="O96" s="19"/>
       <c r="P96" s="19"/>
-      <c r="Q96" s="16"/>
-    </row>
-    <row r="97" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>
       <c r="B97" s="16"/>
       <c r="C97" s="16"/>
@@ -3534,9 +3436,8 @@
       <c r="N97" s="18"/>
       <c r="O97" s="19"/>
       <c r="P97" s="19"/>
-      <c r="Q97" s="16"/>
-    </row>
-    <row r="98" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="16"/>
       <c r="B98" s="16"/>
       <c r="C98" s="16"/>
@@ -3553,9 +3454,8 @@
       <c r="N98" s="18"/>
       <c r="O98" s="19"/>
       <c r="P98" s="19"/>
-      <c r="Q98" s="16"/>
-    </row>
-    <row r="99" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="16"/>
       <c r="B99" s="16"/>
       <c r="C99" s="16"/>
@@ -3572,9 +3472,8 @@
       <c r="N99" s="18"/>
       <c r="O99" s="19"/>
       <c r="P99" s="19"/>
-      <c r="Q99" s="16"/>
-    </row>
-    <row r="100" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="16"/>
       <c r="B100" s="16"/>
       <c r="C100" s="16"/>
@@ -3591,9 +3490,8 @@
       <c r="N100" s="18"/>
       <c r="O100" s="19"/>
       <c r="P100" s="19"/>
-      <c r="Q100" s="16"/>
-    </row>
-    <row r="101" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="16"/>
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
@@ -3610,9 +3508,8 @@
       <c r="N101" s="18"/>
       <c r="O101" s="19"/>
       <c r="P101" s="19"/>
-      <c r="Q101" s="16"/>
-    </row>
-    <row r="102" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="16"/>
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
@@ -3629,9 +3526,8 @@
       <c r="N102" s="18"/>
       <c r="O102" s="19"/>
       <c r="P102" s="19"/>
-      <c r="Q102" s="16"/>
-    </row>
-    <row r="103" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="16"/>
       <c r="B103" s="16"/>
       <c r="C103" s="16"/>
@@ -3648,9 +3544,8 @@
       <c r="N103" s="18"/>
       <c r="O103" s="19"/>
       <c r="P103" s="19"/>
-      <c r="Q103" s="16"/>
-    </row>
-    <row r="104" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="16"/>
       <c r="B104" s="16"/>
       <c r="C104" s="16"/>
@@ -3667,9 +3562,8 @@
       <c r="N104" s="18"/>
       <c r="O104" s="19"/>
       <c r="P104" s="19"/>
-      <c r="Q104" s="16"/>
-    </row>
-    <row r="105" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="16"/>
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
@@ -3686,9 +3580,8 @@
       <c r="N105" s="18"/>
       <c r="O105" s="19"/>
       <c r="P105" s="19"/>
-      <c r="Q105" s="16"/>
-    </row>
-    <row r="106" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="16"/>
       <c r="B106" s="16"/>
       <c r="C106" s="16"/>
@@ -3705,9 +3598,8 @@
       <c r="N106" s="18"/>
       <c r="O106" s="19"/>
       <c r="P106" s="19"/>
-      <c r="Q106" s="16"/>
-    </row>
-    <row r="107" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="16"/>
       <c r="B107" s="16"/>
       <c r="C107" s="16"/>
@@ -3724,9 +3616,8 @@
       <c r="N107" s="18"/>
       <c r="O107" s="19"/>
       <c r="P107" s="19"/>
-      <c r="Q107" s="16"/>
-    </row>
-    <row r="108" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="16"/>
       <c r="B108" s="16"/>
       <c r="C108" s="16"/>
@@ -3743,9 +3634,8 @@
       <c r="N108" s="18"/>
       <c r="O108" s="19"/>
       <c r="P108" s="19"/>
-      <c r="Q108" s="16"/>
-    </row>
-    <row r="109" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="16"/>
       <c r="B109" s="16"/>
       <c r="C109" s="16"/>
@@ -3762,9 +3652,8 @@
       <c r="N109" s="18"/>
       <c r="O109" s="19"/>
       <c r="P109" s="19"/>
-      <c r="Q109" s="16"/>
-    </row>
-    <row r="110" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="16"/>
       <c r="B110" s="16"/>
       <c r="C110" s="16"/>
@@ -3781,9 +3670,8 @@
       <c r="N110" s="18"/>
       <c r="O110" s="19"/>
       <c r="P110" s="19"/>
-      <c r="Q110" s="16"/>
-    </row>
-    <row r="111" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="16"/>
       <c r="B111" s="16"/>
       <c r="C111" s="16"/>
@@ -3800,9 +3688,8 @@
       <c r="N111" s="18"/>
       <c r="O111" s="19"/>
       <c r="P111" s="19"/>
-      <c r="Q111" s="16"/>
-    </row>
-    <row r="112" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="16"/>
       <c r="B112" s="16"/>
       <c r="C112" s="16"/>
@@ -3819,9 +3706,8 @@
       <c r="N112" s="18"/>
       <c r="O112" s="19"/>
       <c r="P112" s="19"/>
-      <c r="Q112" s="16"/>
-    </row>
-    <row r="113" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="16"/>
       <c r="C113" s="16"/>
@@ -3838,9 +3724,8 @@
       <c r="N113" s="18"/>
       <c r="O113" s="19"/>
       <c r="P113" s="19"/>
-      <c r="Q113" s="16"/>
-    </row>
-    <row r="114" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="16"/>
       <c r="B114" s="16"/>
       <c r="C114" s="16"/>
@@ -3857,9 +3742,8 @@
       <c r="N114" s="18"/>
       <c r="O114" s="19"/>
       <c r="P114" s="19"/>
-      <c r="Q114" s="16"/>
-    </row>
-    <row r="115" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="16"/>
       <c r="B115" s="16"/>
       <c r="C115" s="16"/>
@@ -3876,9 +3760,8 @@
       <c r="N115" s="18"/>
       <c r="O115" s="19"/>
       <c r="P115" s="19"/>
-      <c r="Q115" s="16"/>
-    </row>
-    <row r="116" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="16"/>
       <c r="B116" s="16"/>
       <c r="C116" s="16"/>
@@ -3895,9 +3778,8 @@
       <c r="N116" s="18"/>
       <c r="O116" s="19"/>
       <c r="P116" s="19"/>
-      <c r="Q116" s="16"/>
-    </row>
-    <row r="117" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="16"/>
       <c r="B117" s="16"/>
       <c r="C117" s="16"/>
@@ -3914,9 +3796,8 @@
       <c r="N117" s="18"/>
       <c r="O117" s="19"/>
       <c r="P117" s="19"/>
-      <c r="Q117" s="16"/>
-    </row>
-    <row r="118" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="16"/>
       <c r="B118" s="16"/>
       <c r="C118" s="16"/>
@@ -3933,9 +3814,8 @@
       <c r="N118" s="18"/>
       <c r="O118" s="19"/>
       <c r="P118" s="19"/>
-      <c r="Q118" s="16"/>
-    </row>
-    <row r="119" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="16"/>
       <c r="B119" s="16"/>
       <c r="C119" s="16"/>
@@ -3952,9 +3832,8 @@
       <c r="N119" s="18"/>
       <c r="O119" s="19"/>
       <c r="P119" s="19"/>
-      <c r="Q119" s="16"/>
-    </row>
-    <row r="120" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="16"/>
       <c r="B120" s="16"/>
       <c r="C120" s="16"/>
@@ -3971,9 +3850,8 @@
       <c r="N120" s="18"/>
       <c r="O120" s="19"/>
       <c r="P120" s="19"/>
-      <c r="Q120" s="16"/>
-    </row>
-    <row r="121" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="16"/>
       <c r="B121" s="16"/>
       <c r="C121" s="16"/>
@@ -3990,9 +3868,8 @@
       <c r="N121" s="18"/>
       <c r="O121" s="19"/>
       <c r="P121" s="19"/>
-      <c r="Q121" s="16"/>
-    </row>
-    <row r="122" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="16"/>
       <c r="B122" s="16"/>
       <c r="C122" s="16"/>
@@ -4009,9 +3886,8 @@
       <c r="N122" s="18"/>
       <c r="O122" s="19"/>
       <c r="P122" s="19"/>
-      <c r="Q122" s="16"/>
-    </row>
-    <row r="123" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="16"/>
       <c r="B123" s="16"/>
       <c r="C123" s="16"/>
@@ -4028,9 +3904,8 @@
       <c r="N123" s="18"/>
       <c r="O123" s="19"/>
       <c r="P123" s="19"/>
-      <c r="Q123" s="16"/>
-    </row>
-    <row r="124" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="16"/>
       <c r="B124" s="16"/>
       <c r="C124" s="16"/>
@@ -4047,9 +3922,8 @@
       <c r="N124" s="18"/>
       <c r="O124" s="19"/>
       <c r="P124" s="19"/>
-      <c r="Q124" s="16"/>
-    </row>
-    <row r="125" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="16"/>
       <c r="B125" s="16"/>
       <c r="C125" s="16"/>
@@ -4066,9 +3940,8 @@
       <c r="N125" s="18"/>
       <c r="O125" s="19"/>
       <c r="P125" s="19"/>
-      <c r="Q125" s="16"/>
-    </row>
-    <row r="126" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="16"/>
       <c r="B126" s="16"/>
       <c r="C126" s="16"/>
@@ -4085,9 +3958,8 @@
       <c r="N126" s="18"/>
       <c r="O126" s="19"/>
       <c r="P126" s="19"/>
-      <c r="Q126" s="16"/>
-    </row>
-    <row r="127" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="16"/>
       <c r="B127" s="16"/>
       <c r="C127" s="16"/>
@@ -4104,9 +3976,8 @@
       <c r="N127" s="18"/>
       <c r="O127" s="19"/>
       <c r="P127" s="19"/>
-      <c r="Q127" s="16"/>
-    </row>
-    <row r="128" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="16"/>
       <c r="B128" s="16"/>
       <c r="C128" s="16"/>
@@ -4123,9 +3994,8 @@
       <c r="N128" s="18"/>
       <c r="O128" s="19"/>
       <c r="P128" s="19"/>
-      <c r="Q128" s="16"/>
-    </row>
-    <row r="129" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="16"/>
       <c r="B129" s="16"/>
       <c r="C129" s="16"/>
@@ -4142,9 +4012,8 @@
       <c r="N129" s="18"/>
       <c r="O129" s="19"/>
       <c r="P129" s="19"/>
-      <c r="Q129" s="16"/>
-    </row>
-    <row r="130" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="16"/>
       <c r="B130" s="16"/>
       <c r="C130" s="16"/>
@@ -4161,9 +4030,8 @@
       <c r="N130" s="18"/>
       <c r="O130" s="19"/>
       <c r="P130" s="19"/>
-      <c r="Q130" s="16"/>
-    </row>
-    <row r="131" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="16"/>
       <c r="B131" s="16"/>
       <c r="C131" s="16"/>
@@ -4180,9 +4048,8 @@
       <c r="N131" s="18"/>
       <c r="O131" s="19"/>
       <c r="P131" s="19"/>
-      <c r="Q131" s="16"/>
-    </row>
-    <row r="132" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="16"/>
       <c r="B132" s="16"/>
       <c r="C132" s="16"/>
@@ -4199,9 +4066,8 @@
       <c r="N132" s="18"/>
       <c r="O132" s="19"/>
       <c r="P132" s="19"/>
-      <c r="Q132" s="16"/>
-    </row>
-    <row r="133" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="16"/>
       <c r="B133" s="16"/>
       <c r="C133" s="16"/>
@@ -4218,9 +4084,8 @@
       <c r="N133" s="18"/>
       <c r="O133" s="19"/>
       <c r="P133" s="19"/>
-      <c r="Q133" s="16"/>
-    </row>
-    <row r="134" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="16"/>
       <c r="B134" s="16"/>
       <c r="C134" s="16"/>
@@ -4237,9 +4102,8 @@
       <c r="N134" s="18"/>
       <c r="O134" s="19"/>
       <c r="P134" s="19"/>
-      <c r="Q134" s="16"/>
-    </row>
-    <row r="135" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="16"/>
       <c r="B135" s="16"/>
       <c r="C135" s="16"/>
@@ -4256,9 +4120,8 @@
       <c r="N135" s="18"/>
       <c r="O135" s="19"/>
       <c r="P135" s="19"/>
-      <c r="Q135" s="16"/>
-    </row>
-    <row r="136" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="16"/>
       <c r="B136" s="16"/>
       <c r="C136" s="16"/>
@@ -4275,9 +4138,8 @@
       <c r="N136" s="18"/>
       <c r="O136" s="19"/>
       <c r="P136" s="19"/>
-      <c r="Q136" s="16"/>
-    </row>
-    <row r="137" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="16"/>
       <c r="B137" s="16"/>
       <c r="C137" s="16"/>
@@ -4294,9 +4156,8 @@
       <c r="N137" s="18"/>
       <c r="O137" s="19"/>
       <c r="P137" s="19"/>
-      <c r="Q137" s="16"/>
-    </row>
-    <row r="138" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="16"/>
       <c r="B138" s="16"/>
       <c r="C138" s="16"/>
@@ -4313,9 +4174,8 @@
       <c r="N138" s="18"/>
       <c r="O138" s="19"/>
       <c r="P138" s="19"/>
-      <c r="Q138" s="16"/>
-    </row>
-    <row r="139" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="16"/>
       <c r="B139" s="16"/>
       <c r="C139" s="16"/>
@@ -4332,9 +4192,8 @@
       <c r="N139" s="18"/>
       <c r="O139" s="19"/>
       <c r="P139" s="19"/>
-      <c r="Q139" s="16"/>
-    </row>
-    <row r="140" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="16"/>
       <c r="B140" s="16"/>
       <c r="C140" s="16"/>
@@ -4351,9 +4210,8 @@
       <c r="N140" s="18"/>
       <c r="O140" s="19"/>
       <c r="P140" s="19"/>
-      <c r="Q140" s="16"/>
-    </row>
-    <row r="141" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="16"/>
       <c r="B141" s="16"/>
       <c r="C141" s="16"/>
@@ -4370,9 +4228,8 @@
       <c r="N141" s="18"/>
       <c r="O141" s="19"/>
       <c r="P141" s="19"/>
-      <c r="Q141" s="16"/>
-    </row>
-    <row r="142" spans="1:17" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:16" s="15" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="16"/>
       <c r="B142" s="16"/>
       <c r="C142" s="16"/>
@@ -4389,20 +4246,19 @@
       <c r="N142" s="18"/>
       <c r="O142" s="19"/>
       <c r="P142" s="19"/>
-      <c r="Q142" s="16"/>
-    </row>
-    <row r="143" spans="1:17" ht="29.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="31" t="s">
-        <v>26</v>
+    </row>
+    <row r="143" spans="1:16" ht="29.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" spans="1:16" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="24.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="146" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="B146" s="75"/>
+      <c r="A146" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="74"/>
     </row>
     <row r="147" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="148" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4420,14 +4276,14 @@
     <mergeCell ref="K7:P7"/>
     <mergeCell ref="A7:J7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B5:D5">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(B5))=0</formula>
+  <conditionalFormatting sqref="B4:D4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:D4">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
-      <formula>LEN(TRIM(B4))=0</formula>
+  <conditionalFormatting sqref="B5:D5">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:G5">
@@ -4470,40 +4326,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="33" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="41.83203125" style="33" customWidth="1"/>
-    <col min="4" max="6" width="20.83203125" style="33" customWidth="1"/>
-    <col min="7" max="7" width="44.83203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.83203125" style="32" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="33"/>
+    <col min="1" max="1" width="3.5" style="32" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" style="32" customWidth="1"/>
+    <col min="4" max="6" width="20.83203125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="44.83203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" style="31" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F1" s="34"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="92"/>
+      <c r="D2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4511,408 +4367,414 @@
     <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
+      <c r="B10" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="2:10" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="92"/>
+      <c r="D12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="38" t="s">
+      <c r="E12" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="F12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="14" spans="2:10" s="38" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="14" spans="2:10" s="39" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="84" t="s">
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="89"/>
+    </row>
+    <row r="15" spans="2:10" s="38" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="86"/>
-    </row>
-    <row r="15" spans="2:10" s="39" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="87" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="96"/>
+    </row>
+    <row r="16" spans="2:10" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+    </row>
+    <row r="17" spans="2:10" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="89"/>
-    </row>
-    <row r="16" spans="2:10" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-    </row>
-    <row r="17" spans="2:10" s="39" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="42" t="s">
+      <c r="H17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="43" t="s">
+    </row>
+    <row r="18" spans="2:10" s="38" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="87" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" s="39" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="84" t="s">
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="89"/>
+    </row>
+    <row r="19" spans="2:10" s="38" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="43">
+        <v>1</v>
+      </c>
+      <c r="C19" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
-    </row>
-    <row r="19" spans="2:10" s="39" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="44">
-        <v>1</v>
-      </c>
-      <c r="C19" s="90" t="s">
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45"/>
+    </row>
+    <row r="20" spans="2:10" s="38" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="43">
+        <v>2</v>
+      </c>
+      <c r="C20" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="46"/>
-    </row>
-    <row r="20" spans="2:10" s="39" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="44">
-        <v>2</v>
-      </c>
-      <c r="C20" s="90" t="s">
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+    </row>
+    <row r="21" spans="2:10" s="38" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="43">
+        <v>3</v>
+      </c>
+      <c r="C21" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="46"/>
-    </row>
-    <row r="21" spans="2:10" s="39" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="44">
-        <v>3</v>
-      </c>
-      <c r="C21" s="90" t="s">
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="82"/>
+      <c r="H21" s="45"/>
+    </row>
+    <row r="22" spans="2:10" s="38" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="43">
+        <v>4</v>
+      </c>
+      <c r="C22" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="92"/>
-      <c r="H21" s="46"/>
-    </row>
-    <row r="22" spans="2:10" s="39" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="44">
-        <v>4</v>
-      </c>
-      <c r="C22" s="97" t="s">
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="45"/>
+    </row>
+    <row r="23" spans="2:10" s="38" customFormat="1" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="43">
+        <v>5</v>
+      </c>
+      <c r="C23" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
-    </row>
-    <row r="23" spans="2:10" s="39" customFormat="1" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="44">
-        <v>5</v>
-      </c>
-      <c r="C23" s="97" t="s">
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="45"/>
+    </row>
+    <row r="24" spans="2:10" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="43">
+        <v>6</v>
+      </c>
+      <c r="C24" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="46"/>
-    </row>
-    <row r="24" spans="2:10" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="44">
-        <v>6</v>
-      </c>
-      <c r="C24" s="90" t="s">
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+    </row>
+    <row r="25" spans="2:10" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="43">
+        <v>7</v>
+      </c>
+      <c r="C25" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-    </row>
-    <row r="25" spans="2:10" ht="50.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="44">
-        <v>7</v>
-      </c>
-      <c r="C25" s="90" t="s">
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="48"/>
+    </row>
+    <row r="26" spans="2:10" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="43">
+        <v>8</v>
+      </c>
+      <c r="C26" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="49"/>
-    </row>
-    <row r="26" spans="2:10" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="44">
-        <v>8</v>
-      </c>
-      <c r="C26" s="93" t="s">
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="48"/>
+    </row>
+    <row r="27" spans="2:10" ht="110" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="51">
+        <v>9</v>
+      </c>
+      <c r="C27" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="49"/>
-    </row>
-    <row r="27" spans="2:10" ht="110" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="52">
-        <v>9</v>
-      </c>
-      <c r="C27" s="96" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="49"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="48"/>
     </row>
     <row r="28" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="33"/>
-      <c r="D28" s="55"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="32"/>
+      <c r="D28" s="54"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="48"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="49"/>
+      <c r="B29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="48"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="49"/>
+      <c r="B30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="48"/>
     </row>
     <row r="83" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="60"/>
-      <c r="B84" s="61"/>
-      <c r="C84" s="62"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="63"/>
-    </row>
-    <row r="90" spans="1:7" s="32" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="33"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
-    </row>
-    <row r="91" spans="1:7" s="32" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="33"/>
-      <c r="C91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="33"/>
-      <c r="F91" s="64"/>
-      <c r="G91" s="65"/>
-    </row>
-    <row r="92" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="66"/>
-      <c r="B92" s="67"/>
-      <c r="C92" s="64"/>
-      <c r="D92" s="64"/>
-      <c r="E92" s="64"/>
-      <c r="F92" s="64"/>
-      <c r="G92" s="65"/>
-    </row>
-    <row r="93" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="68"/>
-      <c r="C93" s="33"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="69"/>
-    </row>
-    <row r="94" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="68"/>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="69"/>
-    </row>
-    <row r="95" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="68"/>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
-      <c r="F95" s="33"/>
-      <c r="G95" s="69"/>
-    </row>
-    <row r="96" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="68"/>
-      <c r="C96" s="33"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="33"/>
-      <c r="F96" s="33"/>
-      <c r="G96" s="69"/>
-    </row>
-    <row r="97" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="68"/>
-      <c r="C97" s="33"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="33"/>
-      <c r="F97" s="33"/>
-      <c r="G97" s="69"/>
-    </row>
-    <row r="98" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="68"/>
-      <c r="C98" s="33"/>
-      <c r="D98" s="33"/>
-      <c r="E98" s="33"/>
-      <c r="F98" s="33"/>
-      <c r="G98" s="69"/>
-    </row>
-    <row r="99" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="68"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="33"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="69"/>
-    </row>
-    <row r="100" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="68"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
-      <c r="F100" s="33"/>
-      <c r="G100" s="69"/>
-    </row>
-    <row r="101" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="68"/>
-      <c r="C101" s="33"/>
-      <c r="D101" s="33"/>
-      <c r="E101" s="33"/>
-      <c r="F101" s="33"/>
-      <c r="G101" s="69"/>
-    </row>
-    <row r="102" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="68"/>
-      <c r="C102" s="33"/>
-      <c r="D102" s="33"/>
-      <c r="E102" s="33"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="69"/>
-    </row>
-    <row r="103" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="68"/>
-      <c r="C103" s="33"/>
-      <c r="D103" s="33"/>
-      <c r="E103" s="33"/>
-      <c r="F103" s="33"/>
-      <c r="G103" s="69"/>
-    </row>
-    <row r="104" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="68"/>
-      <c r="C104" s="33"/>
-      <c r="D104" s="33"/>
-      <c r="E104" s="33"/>
-      <c r="F104" s="33"/>
-      <c r="G104" s="69"/>
-    </row>
-    <row r="105" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="68"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="33"/>
-      <c r="E105" s="33"/>
-      <c r="F105" s="33"/>
-      <c r="G105" s="69"/>
-    </row>
-    <row r="106" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="68"/>
-      <c r="C106" s="33"/>
-      <c r="D106" s="33"/>
-      <c r="E106" s="33"/>
-      <c r="F106" s="33"/>
-      <c r="G106" s="69"/>
-    </row>
-    <row r="107" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="68"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="33"/>
-      <c r="E107" s="33"/>
-      <c r="F107" s="33"/>
-      <c r="G107" s="69"/>
-    </row>
-    <row r="108" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="68"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="33"/>
-      <c r="E108" s="33"/>
-      <c r="F108" s="33"/>
-      <c r="G108" s="69"/>
-    </row>
-    <row r="109" spans="1:7" s="32" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="70"/>
-      <c r="B109" s="71"/>
-      <c r="C109" s="72"/>
-      <c r="D109" s="72"/>
-      <c r="E109" s="72"/>
-      <c r="F109" s="72"/>
-      <c r="G109" s="73"/>
+      <c r="A84" s="59"/>
+      <c r="B84" s="60"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="62"/>
+    </row>
+    <row r="90" spans="1:7" s="31" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
+    </row>
+    <row r="91" spans="1:7" s="31" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="32"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="63"/>
+      <c r="G91" s="64"/>
+    </row>
+    <row r="92" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="65"/>
+      <c r="B92" s="66"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="63"/>
+      <c r="G92" s="64"/>
+    </row>
+    <row r="93" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="67"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="32"/>
+      <c r="G93" s="68"/>
+    </row>
+    <row r="94" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="67"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="68"/>
+    </row>
+    <row r="95" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="67"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="68"/>
+    </row>
+    <row r="96" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="67"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="68"/>
+    </row>
+    <row r="97" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="67"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="68"/>
+    </row>
+    <row r="98" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="67"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="68"/>
+    </row>
+    <row r="99" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="67"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="32"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
+      <c r="G99" s="68"/>
+    </row>
+    <row r="100" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="67"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="68"/>
+    </row>
+    <row r="101" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="67"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="68"/>
+    </row>
+    <row r="102" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="67"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="32"/>
+      <c r="G102" s="68"/>
+    </row>
+    <row r="103" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="67"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="68"/>
+    </row>
+    <row r="104" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="67"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="68"/>
+    </row>
+    <row r="105" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="67"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="32"/>
+      <c r="G105" s="68"/>
+    </row>
+    <row r="106" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="67"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="68"/>
+    </row>
+    <row r="107" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="67"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="32"/>
+      <c r="G107" s="68"/>
+    </row>
+    <row r="108" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="67"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="32"/>
+      <c r="E108" s="32"/>
+      <c r="F108" s="32"/>
+      <c r="G108" s="68"/>
+    </row>
+    <row r="109" spans="1:7" s="31" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="69"/>
+      <c r="B109" s="70"/>
+      <c r="C109" s="71"/>
+      <c r="D109" s="71"/>
+      <c r="E109" s="71"/>
+      <c r="F109" s="71"/>
+      <c r="G109" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C26:F26"/>
@@ -4923,12 +4785,6 @@
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4947,12 +4803,12 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -4962,7 +4818,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
@@ -4987,12 +4843,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>